<commit_message>
p2u error kunjungan online
</commit_message>
<xml_diff>
--- a/Filexel/Keamanan.xlsx
+++ b/Filexel/Keamanan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16940"/>
+    <workbookView windowWidth="28000" windowHeight="13760"/>
   </bookViews>
   <sheets>
     <sheet name="DaftarLaluLintas_Input" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
   <si>
     <t>Drpdownsearch</t>
   </si>
@@ -1087,10 +1087,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
@@ -1180,7 +1180,7 @@
         <v>9</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" ht="15.6" spans="1:6">
@@ -1188,7 +1188,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -1200,68 +1200,32 @@
         <v>9</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" ht="15.6" spans="1:6">
-      <c r="A6" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" ht="15.6" spans="1:6">
-      <c r="A7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" ht="15.6" spans="1:6">
-      <c r="A8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9"/>
@@ -1294,6 +1258,302 @@
       <c r="D12"/>
       <c r="E12"/>
       <c r="F12"/>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37"/>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38"/>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39"/>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40"/>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41"/>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
daftar lalu lintas excel
</commit_message>
<xml_diff>
--- a/Filexel/Keamanan.xlsx
+++ b/Filexel/Keamanan.xlsx
@@ -4,21 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16740"/>
+    <workbookView windowHeight="16760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="DaftarLaluLintas_Input" sheetId="1" r:id="rId1"/>
     <sheet name="DaftarLaluLintas_ubah" sheetId="2" r:id="rId2"/>
+    <sheet name="DaftarLaluLintas_Index" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="19">
-  <si>
-    <t>Drpdownsearch</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
   <si>
     <t>Nama</t>
   </si>
@@ -35,43 +33,61 @@
     <t>Deskripsi</t>
   </si>
   <si>
+    <t>PengawalInternal</t>
+  </si>
+  <si>
+    <t>PengawalExternal</t>
+  </si>
+  <si>
     <t>ALYA BINTI GONGYOO</t>
   </si>
   <si>
     <t>Cuti Bersyarat</t>
   </si>
   <si>
-    <t>17/05/2017'</t>
-  </si>
-  <si>
-    <t>20/05/2017'</t>
+    <t>17/12/2022'</t>
+  </si>
+  <si>
+    <t>29/11/2022 12:00:00'</t>
+  </si>
+  <si>
+    <t>Robi</t>
+  </si>
+  <si>
+    <t>rehan</t>
   </si>
   <si>
     <t>sanihsan</t>
   </si>
   <si>
+    <t>READ BARIS</t>
+  </si>
+  <si>
     <t>WILLLD BINTI eko cah cah ge</t>
   </si>
   <si>
     <t>MAP</t>
   </si>
   <si>
-    <t>'05/05/2017</t>
-  </si>
-  <si>
-    <t>24/05/2017'</t>
-  </si>
-  <si>
     <t>Masih ada Perkara nih doi</t>
   </si>
   <si>
     <t>Mutasi Keluar</t>
   </si>
   <si>
-    <t>'01/05/2017</t>
-  </si>
-  <si>
     <t>Mutasi Keluar nih Doi</t>
+  </si>
+  <si>
+    <t>filterColumn</t>
+  </si>
+  <si>
+    <t>nomorInduk</t>
+  </si>
+  <si>
+    <t>namaLengkap</t>
+  </si>
+  <si>
+    <t>EYONO BIN CAS</t>
   </si>
 </sst>
 </file>
@@ -80,8 +96,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="22">
@@ -115,7 +131,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -130,6 +154,42 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -138,34 +198,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -174,18 +206,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,14 +237,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -212,7 +244,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -220,37 +258,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -259,19 +275,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCEFED5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -283,7 +359,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,13 +395,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -313,139 +467,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -474,11 +496,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -498,11 +535,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,21 +565,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -551,165 +579,159 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -719,19 +741,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" quotePrefix="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1080,120 +1102,141 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F49"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.0078125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="18.859375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="21.1484375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.859375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="21.4296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="15.4296875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.0078125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.859375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.1484375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="16.859375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="21.4296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="23.6875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="14.96875" customWidth="1"/>
+    <col min="8" max="8" width="26.953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="19.5" customHeight="1" spans="1:8">
+      <c r="A1"/>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="2" ht="19.5" customHeight="1" spans="1:8">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="2:8">
+      <c r="B3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" ht="15.6" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="F3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" ht="15.6" spans="2:8">
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="F4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" ht="15.6" spans="2:8">
+      <c r="B5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="D5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" ht="15.6" spans="1:6">
-      <c r="A5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1559,84 +1602,159 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="14.1484375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="32.1484375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="29.859375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.1484375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.4296875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="42.0078125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.1484375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="32.1484375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="29.859375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="27.1484375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="32.4296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="42.0078125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:6">
       <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="3" t="s">
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="2:6">
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5">
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5">
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="14.9765625" customWidth="1"/>
+    <col min="2" max="2" width="23.296875" customWidth="1"/>
+    <col min="3" max="3" width="26.296875" customWidth="1"/>
+    <col min="4" max="4" width="16.015625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>50120</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>50120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit daftar lalu lintas
</commit_message>
<xml_diff>
--- a/Filexel/Keamanan.xlsx
+++ b/Filexel/Keamanan.xlsx
@@ -4,19 +4,23 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760"/>
+    <workbookView windowHeight="16760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DaftarLaluLintas_Input" sheetId="1" r:id="rId1"/>
     <sheet name="DaftarLaluLintas_ubah" sheetId="2" r:id="rId2"/>
     <sheet name="DaftarLaluLintas_Index" sheetId="3" r:id="rId3"/>
+    <sheet name="DaftarLaluLintas_CariIdentitas" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="47">
+  <si>
+    <t>READ BARIS</t>
+  </si>
   <si>
     <t>Nama</t>
   </si>
@@ -42,52 +46,118 @@
     <t>ALYA BINTI GONGYOO</t>
   </si>
   <si>
+    <t>Cuti Menjelang Bebas</t>
+  </si>
+  <si>
+    <t>17/12/2022'</t>
+  </si>
+  <si>
+    <t>29/11/2022 12:00:00'</t>
+  </si>
+  <si>
+    <t>Robi</t>
+  </si>
+  <si>
+    <t>rehan</t>
+  </si>
+  <si>
+    <t>sanihsan</t>
+  </si>
+  <si>
     <t>Cuti Bersyarat</t>
   </si>
   <si>
-    <t>17/12/2022'</t>
-  </si>
-  <si>
-    <t>29/11/2022 12:00:00'</t>
-  </si>
-  <si>
-    <t>Robi</t>
-  </si>
-  <si>
-    <t>rehan</t>
-  </si>
-  <si>
-    <t>sanihsan</t>
-  </si>
-  <si>
-    <t>READ BARIS</t>
+    <t>Asimilasi</t>
+  </si>
+  <si>
+    <t>Bebas dari Dakwaan</t>
+  </si>
+  <si>
+    <t>Bebas dari Tuntutan</t>
+  </si>
+  <si>
+    <t>NamaEdit</t>
+  </si>
+  <si>
+    <t>noSK</t>
+  </si>
+  <si>
+    <t>JenisKeluarEdit</t>
+  </si>
+  <si>
+    <t>TanggalKeluarEdit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TanggalHarusKembaliEdit  </t>
+  </si>
+  <si>
+    <t>DeskripsiEdit</t>
+  </si>
+  <si>
+    <t>PengawalInternalEdit</t>
+  </si>
+  <si>
+    <t>PengawalExternalEdit</t>
+  </si>
+  <si>
+    <t>Wildan Cahyono</t>
+  </si>
+  <si>
+    <t>SK/001/DIV</t>
+  </si>
+  <si>
+    <t>EDIT</t>
+  </si>
+  <si>
+    <t>EYONO BIN CAS</t>
+  </si>
+  <si>
+    <t>SK/002/DIV</t>
+  </si>
+  <si>
+    <t>SK/003/DIV</t>
+  </si>
+  <si>
+    <t>SK/004/DIV</t>
+  </si>
+  <si>
+    <t>SK/005/DIV</t>
+  </si>
+  <si>
+    <t>SK/006/DIV</t>
+  </si>
+  <si>
+    <t>SK/007/DIV</t>
+  </si>
+  <si>
+    <t>SK/008/DIV</t>
+  </si>
+  <si>
+    <t>SK/009/DIV</t>
+  </si>
+  <si>
+    <t>filterColumn</t>
+  </si>
+  <si>
+    <t>nomorInduk</t>
+  </si>
+  <si>
+    <t>namaLengkap</t>
+  </si>
+  <si>
+    <t>nomorReg</t>
+  </si>
+  <si>
+    <t>jenisKejahatan</t>
   </si>
   <si>
     <t>WILLLD BINTI eko cah cah ge</t>
   </si>
   <si>
-    <t>MAP</t>
-  </si>
-  <si>
-    <t>Masih ada Perkara nih doi</t>
-  </si>
-  <si>
-    <t>Mutasi Keluar</t>
-  </si>
-  <si>
-    <t>Mutasi Keluar nih Doi</t>
-  </si>
-  <si>
-    <t>filterColumn</t>
-  </si>
-  <si>
-    <t>nomorInduk</t>
-  </si>
-  <si>
-    <t>namaLengkap</t>
-  </si>
-  <si>
-    <t>EYONO BIN CAS</t>
+    <t>Korupsi</t>
+  </si>
+  <si>
+    <t>nama</t>
   </si>
 </sst>
 </file>
@@ -95,15 +165,22 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -116,10 +193,13 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="10.5"/>
-      <color rgb="FF606266"/>
-      <name val="Roboto"/>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -138,8 +218,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -155,29 +242,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -190,19 +271,26 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -223,7 +311,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -238,35 +340,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -281,6 +361,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFCEFED5"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -293,25 +379,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -323,7 +511,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,146 +557,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -482,16 +568,162 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -507,6 +739,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -531,21 +772,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -579,169 +805,175 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -750,10 +982,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1104,15 +1362,15 @@
   </sheetPr>
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="14.0078125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18.859375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.1484375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.46875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="30.203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="16.859375" style="3" customWidth="1"/>
     <col min="5" max="5" width="21.4296875" style="3" customWidth="1"/>
     <col min="6" max="6" width="23.6875" style="2" customWidth="1"/>
@@ -1121,163 +1379,248 @@
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A1"/>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F1" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G1" s="14" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="23" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A2" s="2">
-        <v>5</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="A2" s="16">
+        <v>3</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="E2" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H2" t="s">
+      <c r="F2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" spans="2:8">
-      <c r="B3" s="5" t="s">
+      <c r="H2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="1:8">
+      <c r="A3" s="17"/>
+      <c r="B3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="17"/>
+      <c r="B4" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="G4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="17"/>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="17"/>
+      <c r="B7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="D7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="E7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="17"/>
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="H3" t="s">
+      <c r="F8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="9" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" ht="15.6" spans="2:8">
-      <c r="B4" s="5" t="s">
+      <c r="H8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="17"/>
+      <c r="B9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="C9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" ht="14.75" spans="1:8">
+      <c r="A10" s="18"/>
+      <c r="B10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="D10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="E10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="H4" t="s">
+      <c r="F10" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="19" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" ht="15.6" spans="2:8">
-      <c r="B5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
-      <c r="D6"/>
-      <c r="E6"/>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7"/>
-      <c r="B7"/>
-      <c r="C7"/>
-      <c r="D7"/>
-      <c r="E7"/>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8"/>
-      <c r="B8"/>
-      <c r="C8"/>
-      <c r="D8"/>
-      <c r="E8"/>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9"/>
-      <c r="B9"/>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10"/>
-      <c r="B10"/>
-      <c r="C10"/>
-      <c r="D10"/>
-      <c r="E10"/>
-      <c r="F10"/>
+      <c r="H10" s="25" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:6">
       <c r="A11"/>
@@ -1355,7 +1698,7 @@
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20"/>
+      <c r="D20" s="21"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
@@ -1363,7 +1706,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21"/>
+      <c r="D21" s="21"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
@@ -1371,7 +1714,7 @@
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22"/>
+      <c r="D22" s="21"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
@@ -1379,7 +1722,7 @@
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23"/>
+      <c r="D23" s="21"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
@@ -1387,7 +1730,7 @@
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24"/>
+      <c r="D24" s="21"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
@@ -1395,7 +1738,7 @@
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25"/>
+      <c r="D25" s="21"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
@@ -1403,7 +1746,7 @@
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26"/>
+      <c r="D26" s="21"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
@@ -1411,7 +1754,7 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27"/>
+      <c r="D27" s="21"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
@@ -1419,7 +1762,7 @@
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28"/>
+      <c r="D28" s="21"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
@@ -1592,6 +1935,11 @@
       <c r="F49"/>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C10">
+      <formula1>"Asimilasi,Cuti Menjelang Bebas,Anak Kembali ke Orang Tua,Cuti Bersyarat,Asimilasi di Rumah,Bebas Biasa,Bebas dari Dakwaan,Bebas dari Tuntutan,Cuti Menjelang Bebas"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1602,13 +1950,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="14.1484375" style="2" customWidth="1"/>
     <col min="2" max="2" width="32.1484375" style="2" customWidth="1"/>
@@ -1616,82 +1964,276 @@
     <col min="4" max="4" width="27.1484375" style="3" customWidth="1"/>
     <col min="5" max="5" width="32.4296875" style="3" customWidth="1"/>
     <col min="6" max="6" width="42.0078125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="23.703125" customWidth="1"/>
+    <col min="8" max="8" width="24.8671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
+    <row r="1" ht="19.5" customHeight="1" spans="1:9">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="B1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" ht="19.5" customHeight="1" spans="1:9">
+      <c r="A2" s="8">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" ht="19.5" customHeight="1" spans="1:6">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" ht="19.5" customHeight="1" spans="1:9">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E3" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="9"/>
+      <c r="B4" s="9"/>
+      <c r="C4" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="9"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="9"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" ht="19.5" customHeight="1" spans="2:6">
-      <c r="B3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="F7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9"/>
+      <c r="C10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="4:5">
-      <c r="D4" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5">
-      <c r="D5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>10</v>
+      <c r="F10" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
+      <formula1>"Asimilasi,Cuti Menjelang Bebas,Anak Kembali ke Orang Tua,Cuti Bersyarat,Asimilasi di Rumah,Bebas Biasa,Bebas dari Dakwaan,Bebas dari Tuntutan,Cuti Menjelang Bebas"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1703,7 +2245,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A1" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1716,16 +2258,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1733,10 +2275,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D2">
         <v>50120</v>
@@ -1744,13 +2286,80 @@
     </row>
     <row r="3" spans="2:4">
       <c r="B3" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D3">
         <v>50120</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N16" sqref="N16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="16.5390625" customWidth="1"/>
+    <col min="2" max="2" width="25.7734375" customWidth="1"/>
+    <col min="4" max="4" width="25.78125" customWidth="1"/>
+    <col min="5" max="5" width="17.578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2">
+        <v>123</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edit portir data from excel
</commit_message>
<xml_diff>
--- a/Filexel/Keamanan.xlsx
+++ b/Filexel/Keamanan.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="16760" activeTab="1"/>
+    <workbookView windowHeight="16760" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="DaftarLaluLintas_Input" sheetId="1" r:id="rId1"/>
     <sheet name="DaftarLaluLintas_Edit" sheetId="2" r:id="rId2"/>
     <sheet name="DaftarLaluLintas_Index" sheetId="3" r:id="rId3"/>
     <sheet name="DaftarLaluLintas_CariIdentitas" sheetId="4" r:id="rId4"/>
+    <sheet name="Portir_SearchDataIndex" sheetId="5" r:id="rId5"/>
+    <sheet name="Portir_KeluarKeamanan" sheetId="6" r:id="rId6"/>
+    <sheet name="Portir_KeluarPortir" sheetId="7" r:id="rId7"/>
+    <sheet name="Portir_MasukPortir" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="68">
   <si>
     <t>READ BARIS</t>
   </si>
@@ -158,6 +162,69 @@
   </si>
   <si>
     <t>nama</t>
+  </si>
+  <si>
+    <t>nama_lengkap</t>
+  </si>
+  <si>
+    <t>nomor_induk</t>
+  </si>
+  <si>
+    <t>NomorSurat</t>
+  </si>
+  <si>
+    <t>Pendaftar</t>
+  </si>
+  <si>
+    <t>semua</t>
+  </si>
+  <si>
+    <t>statusColumn</t>
+  </si>
+  <si>
+    <t>Nomor Surat Penetapan</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>NS1005</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Keluar Keamanan</t>
+  </si>
+  <si>
+    <t>nomor induk</t>
+  </si>
+  <si>
+    <t>NS1006</t>
+  </si>
+  <si>
+    <t>NS1007</t>
+  </si>
+  <si>
+    <t>Keluar Portir</t>
+  </si>
+  <si>
+    <t>NS1008</t>
+  </si>
+  <si>
+    <t>Masuk Portir</t>
+  </si>
+  <si>
+    <t>NS1009</t>
+  </si>
+  <si>
+    <t>NS1010</t>
+  </si>
+  <si>
+    <t>KeluarKeamanan</t>
+  </si>
+  <si>
+    <t>NamaWbp</t>
   </si>
 </sst>
 </file>
@@ -166,9 +233,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -202,14 +269,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -226,48 +285,10 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,7 +301,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -289,6 +310,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -311,14 +339,68 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -330,21 +412,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -379,6 +446,132 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -391,7 +584,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,145 +608,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -551,14 +624,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -567,16 +634,149 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color auto="1"/>
       </left>
       <right style="thin">
         <color auto="1"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color auto="1"/>
       </top>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -603,126 +803,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -739,15 +819,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -825,193 +896,212 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1363,262 +1453,262 @@
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.0078125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.46875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.859375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="21.4296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="23.6875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.0078125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.46875" style="12" customWidth="1"/>
+    <col min="3" max="3" width="30.203125" style="12" customWidth="1"/>
+    <col min="4" max="4" width="16.859375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="21.4296875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="23.6875" style="12" customWidth="1"/>
     <col min="7" max="7" width="14.96875" customWidth="1"/>
     <col min="8" max="8" width="26.953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="33" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A2" s="16">
+      <c r="A2" s="26">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A3" s="17"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="17"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="17"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="27"/>
+      <c r="B5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="17"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="27"/>
+      <c r="B6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="17"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="27"/>
+      <c r="B8" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="17"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="27"/>
+      <c r="B9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="34" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.75" spans="1:8">
-      <c r="A10" s="18"/>
-      <c r="B10" s="19" t="s">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="20" t="s">
+      <c r="E10" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="19" t="s">
+      <c r="F10" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="19" t="s">
+      <c r="G10" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="35" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1698,7 +1788,7 @@
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20" s="21"/>
+      <c r="D20" s="31"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
@@ -1706,7 +1796,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" s="21"/>
+      <c r="D21" s="31"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
@@ -1714,7 +1804,7 @@
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="21"/>
+      <c r="D22" s="31"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
@@ -1722,7 +1812,7 @@
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="21"/>
+      <c r="D23" s="31"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
@@ -1730,7 +1820,7 @@
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="21"/>
+      <c r="D24" s="31"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
@@ -1738,7 +1828,7 @@
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25" s="21"/>
+      <c r="D25" s="31"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
@@ -1746,7 +1836,7 @@
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="21"/>
+      <c r="D26" s="31"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
@@ -1754,7 +1844,7 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="21"/>
+      <c r="D27" s="31"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
@@ -1762,7 +1852,7 @@
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28" s="21"/>
+      <c r="D28" s="31"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
@@ -1952,293 +2042,293 @@
   </sheetPr>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.1484375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.1484375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.859375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.1484375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="32.4296875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="42.0078125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="14.1484375" style="12" customWidth="1"/>
+    <col min="2" max="2" width="32.1484375" style="12" customWidth="1"/>
+    <col min="3" max="3" width="29.859375" style="12" customWidth="1"/>
+    <col min="4" max="4" width="27.1484375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="32.4296875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="42.0078125" style="12" customWidth="1"/>
     <col min="7" max="7" width="23.703125" customWidth="1"/>
     <col min="8" max="8" width="24.8671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="14" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A2" s="8">
+      <c r="A2" s="18">
         <v>3</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A3" s="9"/>
-      <c r="B3" s="9" t="s">
+      <c r="A3" s="19"/>
+      <c r="B3" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="9"/>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="9" t="s">
+      <c r="I4" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="9"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="9"/>
-      <c r="B6" s="9" t="s">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="12" t="s">
+      <c r="E6" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="9"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="12" t="s">
+      <c r="F7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="9"/>
-      <c r="B8" s="9" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="9" t="s">
+      <c r="I8" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="9"/>
-      <c r="B9" s="9" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="19" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="9"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="E10" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="19" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2380,4 +2470,315 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:H14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
+  <cols>
+    <col min="1" max="1" width="15.75" customWidth="1"/>
+    <col min="2" max="2" width="25.2578125" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.578125" customWidth="1"/>
+    <col min="6" max="6" width="13.5390625" customWidth="1"/>
+    <col min="7" max="7" width="25.78125" customWidth="1"/>
+    <col min="8" max="8" width="17.6953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="4">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5">
+        <v>50120</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="4"/>
+      <c r="B3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="5">
+        <v>50121</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="5">
+        <v>50122</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="5">
+        <v>50123</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="4"/>
+      <c r="B6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="5">
+        <v>50124</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" ht="14.75" spans="1:8">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
+        <v>50125</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="5">
+        <v>14</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7">
+      <formula1>"Masuk Portir,Keluar Keamanan,Keluar Portir"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="13.8046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
edit blok dan kamar
</commit_message>
<xml_diff>
--- a/Filexel/Keamanan.xlsx
+++ b/Filexel/Keamanan.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="260">
   <si>
     <t>READ BARIS</t>
   </si>
@@ -719,7 +719,7 @@
     <t>lamaHuni</t>
   </si>
   <si>
-    <t>Blok mapen new</t>
+    <t>Blok Naling B</t>
   </si>
   <si>
     <t>Laki-laki</t>
@@ -820,10 +820,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -863,39 +863,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -909,8 +878,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -926,20 +910,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -949,6 +925,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -971,13 +955,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -985,7 +962,38 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -998,16 +1006,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="43">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1034,13 +1034,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.6"/>
+        <fgColor theme="0" tint="-0.25"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,25 +1076,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,7 +1106,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1130,13 +1142,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1148,31 +1214,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,67 +1226,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1256,12 +1250,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -1472,15 +1466,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -1490,10 +1480,8 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
       </top>
       <bottom style="thin">
@@ -1505,13 +1493,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
+      <right/>
+      <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -1520,6 +1506,51 @@
       <left style="medium">
         <color auto="1"/>
       </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="medium">
         <color auto="1"/>
       </right>
@@ -1530,10 +1561,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="thin">
         <color auto="1"/>
       </top>
@@ -1543,33 +1574,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1585,6 +1600,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1615,17 +1654,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1633,144 +1666,129 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="27" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="25" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="24" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="30" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1779,29 +1797,29 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1816,77 +1834,73 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2243,56 +2257,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="14.0078125" style="58" customWidth="1"/>
-    <col min="2" max="2" width="27.46875" style="58" customWidth="1"/>
-    <col min="3" max="3" width="30.203125" style="58" customWidth="1"/>
-    <col min="4" max="4" width="16.859375" style="59" customWidth="1"/>
-    <col min="5" max="5" width="21.4296875" style="59" customWidth="1"/>
-    <col min="6" max="6" width="23.6875" style="58" customWidth="1"/>
+    <col min="1" max="1" width="14.0078125" style="54" customWidth="1"/>
+    <col min="2" max="2" width="27.46875" style="54" customWidth="1"/>
+    <col min="3" max="3" width="30.203125" style="54" customWidth="1"/>
+    <col min="4" max="4" width="16.859375" style="55" customWidth="1"/>
+    <col min="5" max="5" width="21.4296875" style="55" customWidth="1"/>
+    <col min="6" max="6" width="23.6875" style="54" customWidth="1"/>
     <col min="7" max="7" width="14.96875" customWidth="1"/>
     <col min="8" max="8" width="26.953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="66" t="s">
+      <c r="D1" s="62" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="66" t="s">
+      <c r="E1" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="70" t="s">
+      <c r="F1" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="43" t="s">
+      <c r="H1" s="39" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A2" s="67">
+      <c r="A2" s="63">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F2" s="8" t="s">
@@ -2301,22 +2315,22 @@
       <c r="G2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" ht="19.5" customHeight="1" spans="1:8">
-      <c r="A3" s="41"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F3" s="8" t="s">
@@ -2325,22 +2339,22 @@
       <c r="G3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="41"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -2349,22 +2363,22 @@
       <c r="G4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="41"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2373,22 +2387,22 @@
       <c r="G5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="41"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F6" s="8" t="s">
@@ -2397,22 +2411,22 @@
       <c r="G6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="41"/>
+      <c r="A7" s="37"/>
       <c r="B7" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F7" s="8" t="s">
@@ -2421,22 +2435,22 @@
       <c r="G7" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="41"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F8" s="8" t="s">
@@ -2445,22 +2459,22 @@
       <c r="G8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="41"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="37" t="s">
+      <c r="D9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="33" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="8" t="s">
@@ -2469,22 +2483,22 @@
       <c r="G9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="15" t="s">
+      <c r="H9" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" ht="14.75" spans="1:8">
-      <c r="A10" s="42"/>
+      <c r="A10" s="38"/>
       <c r="B10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="68" t="s">
+      <c r="E10" s="64" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="10" t="s">
@@ -2493,7 +2507,7 @@
       <c r="G10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="44" t="s">
+      <c r="H10" s="40" t="s">
         <v>13</v>
       </c>
     </row>
@@ -2573,7 +2587,7 @@
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
-      <c r="D20" s="69"/>
+      <c r="D20" s="65"/>
       <c r="E20"/>
       <c r="F20"/>
     </row>
@@ -2581,7 +2595,7 @@
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
-      <c r="D21" s="69"/>
+      <c r="D21" s="65"/>
       <c r="E21"/>
       <c r="F21"/>
     </row>
@@ -2589,7 +2603,7 @@
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
-      <c r="D22" s="69"/>
+      <c r="D22" s="65"/>
       <c r="E22"/>
       <c r="F22"/>
     </row>
@@ -2597,7 +2611,7 @@
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
-      <c r="D23" s="69"/>
+      <c r="D23" s="65"/>
       <c r="E23"/>
       <c r="F23"/>
     </row>
@@ -2605,7 +2619,7 @@
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
-      <c r="D24" s="69"/>
+      <c r="D24" s="65"/>
       <c r="E24"/>
       <c r="F24"/>
     </row>
@@ -2613,7 +2627,7 @@
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
-      <c r="D25" s="69"/>
+      <c r="D25" s="65"/>
       <c r="E25"/>
       <c r="F25"/>
     </row>
@@ -2621,7 +2635,7 @@
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
-      <c r="D26" s="69"/>
+      <c r="D26" s="65"/>
       <c r="E26"/>
       <c r="F26"/>
     </row>
@@ -2629,7 +2643,7 @@
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
-      <c r="D27" s="69"/>
+      <c r="D27" s="65"/>
       <c r="E27"/>
       <c r="F27"/>
     </row>
@@ -2637,7 +2651,7 @@
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
-      <c r="D28" s="69"/>
+      <c r="D28" s="65"/>
       <c r="E28"/>
       <c r="F28"/>
     </row>
@@ -3357,33 +3371,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9">
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="35" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="40" t="s">
+      <c r="C1" s="36" t="s">
         <v>156</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="D1" s="36" t="s">
         <v>157</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="E1" s="36" t="s">
         <v>158</v>
       </c>
-      <c r="F1" s="40" t="s">
+      <c r="F1" s="36" t="s">
         <v>159</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="40" t="s">
+      <c r="H1" s="36" t="s">
         <v>160</v>
       </c>
-      <c r="I1" s="43" t="s">
+      <c r="I1" s="39" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="2" spans="2:9">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="37" t="s">
         <v>157</v>
       </c>
       <c r="C2" s="8" t="s">
@@ -3404,12 +3418,12 @@
       <c r="H2" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="3" spans="2:9">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="37" t="s">
         <v>167</v>
       </c>
       <c r="C3" s="8" t="s">
@@ -3428,12 +3442,12 @@
       <c r="H3" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="14" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="2:9">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="37" t="s">
         <v>159</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -3452,12 +3466,12 @@
       <c r="H4" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="14" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="5" ht="14.75" spans="2:9">
-      <c r="B5" s="42" t="s">
+      <c r="B5" s="38" t="s">
         <v>158</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -3476,7 +3490,7 @@
       <c r="H5" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="I5" s="44" t="s">
+      <c r="I5" s="40" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3485,11 +3499,11 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5">
       <formula1>"status,blok,jumlahlantai,semua,tipeblok"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
+      <formula1>"status,blok,jumlahlantai,semua"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>"Mapenaling,Umum,Tutup Sunyi,Isolasi"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6">
-      <formula1>"status,blok,jumlahlantai,semua"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5 D6 F6 D2:D4 H2:H5">
       <formula1>"Diizinkan,Perbaikan,Ditolak,Dalam Proses"</formula1>
@@ -3573,7 +3587,7 @@
       <c r="I2" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K2" t="s">
@@ -3605,7 +3619,7 @@
       <c r="I3" t="s">
         <v>190</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="33" t="s">
         <v>191</v>
       </c>
       <c r="K3" t="s">
@@ -3637,7 +3651,7 @@
       <c r="I4" t="s">
         <v>193</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="33" t="s">
         <v>194</v>
       </c>
       <c r="K4" t="s">
@@ -3669,7 +3683,7 @@
       <c r="I5" t="s">
         <v>195</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="33" t="s">
         <v>196</v>
       </c>
       <c r="K5" t="s">
@@ -3707,31 +3721,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:10">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="31" t="s">
         <v>197</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="31" t="s">
         <v>167</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="31" t="s">
         <v>201</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="I1" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="31" t="s">
         <v>181</v>
       </c>
     </row>
@@ -3853,11 +3867,11 @@
     </row>
   </sheetData>
   <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
+      <formula1>"Diizinkan,Dalam Proses,Perbaikan,Ditolak,Semua"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I5">
       <formula1>"Diizinkan,Perbaikan,Ditolak,Dalam Proses"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
-      <formula1>"Diizinkan,Dalam Proses,Perbaikan,Ditolak,Semua"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B5">
       <formula1>"semua,No Registrasi,Nama,Perkara,Blok,Kamar,Tgl Masuk,Tgl Ekspirasi,Status"</formula1>
@@ -3893,34 +3907,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11">
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="31" t="s">
         <v>202</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="K1" s="31" t="s">
         <v>213</v>
       </c>
     </row>
@@ -3949,7 +3963,7 @@
       <c r="I2" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="J2" s="37" t="s">
+      <c r="J2" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K2" s="8" t="s">
@@ -3981,7 +3995,7 @@
       <c r="I3" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="J3" s="37" t="s">
+      <c r="J3" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K3" s="8" t="s">
@@ -4013,7 +4027,7 @@
       <c r="I4" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="J4" s="37" t="s">
+      <c r="J4" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K4" s="8" t="s">
@@ -4045,7 +4059,7 @@
       <c r="I5" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="33" t="s">
         <v>10</v>
       </c>
       <c r="K5" s="8" t="s">
@@ -4074,8 +4088,8 @@
   <sheetPr/>
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:L5"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="4"/>
@@ -4097,267 +4111,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33" t="s">
+      <c r="B1" s="8"/>
+      <c r="C1" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="8" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="8" t="s">
         <v>220</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="L1" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="M1" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="N1" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="O1" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="P1" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="Q1" s="8" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="33">
+      <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="33" t="s">
+      <c r="E2" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="34" t="s">
+      <c r="F2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="35">
+      <c r="G2" s="32">
         <v>2</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="J2" s="33">
+      <c r="J2" s="8">
         <v>10</v>
       </c>
-      <c r="K2" s="33">
+      <c r="K2" s="8">
         <v>1</v>
       </c>
-      <c r="L2" s="33">
+      <c r="L2" s="8">
         <v>10</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>45</v>
       </c>
-      <c r="O2" s="33">
+      <c r="O2" s="8">
         <v>30</v>
       </c>
-      <c r="P2" s="33" t="s">
+      <c r="P2" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="Q2" s="33">
+      <c r="Q2" s="8">
         <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="33">
+      <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E3" s="33" t="s">
+      <c r="E3" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="G3" s="35">
+      <c r="G3" s="32">
         <v>1</v>
       </c>
-      <c r="H3" s="33" t="s">
+      <c r="H3" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="J3" s="33">
+      <c r="J3" s="8">
         <v>15</v>
       </c>
-      <c r="K3" s="33">
+      <c r="K3" s="8">
         <v>2</v>
       </c>
-      <c r="L3" s="33">
+      <c r="L3" s="8">
         <v>15</v>
       </c>
-      <c r="M3" s="33" t="s">
+      <c r="M3" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="N3" s="34" t="s">
+      <c r="N3" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="O3" s="33">
+      <c r="O3" s="8">
         <v>33</v>
       </c>
-      <c r="P3" s="33" t="s">
+      <c r="P3" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="Q3" s="33">
+      <c r="Q3" s="8">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="33">
+      <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33" t="s">
+      <c r="B4" s="8"/>
+      <c r="C4" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="E4" s="33" t="s">
+      <c r="E4" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="G4" s="35">
+      <c r="G4" s="32">
         <v>3</v>
       </c>
-      <c r="H4" s="33" t="s">
+      <c r="H4" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="J4" s="33">
+      <c r="J4" s="8">
         <v>14</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="8">
         <v>3</v>
       </c>
-      <c r="L4" s="33">
+      <c r="L4" s="8">
         <v>14</v>
       </c>
-      <c r="M4" s="33" t="s">
+      <c r="M4" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="N4" s="34" t="s">
+      <c r="N4" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="O4" s="33">
+      <c r="O4" s="8">
         <v>43</v>
       </c>
-      <c r="P4" s="33" t="s">
+      <c r="P4" s="8" t="s">
         <v>233</v>
       </c>
-      <c r="Q4" s="33">
+      <c r="Q4" s="8">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="33">
+      <c r="A5" s="8">
         <v>4</v>
       </c>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="D5" s="33" t="s">
+      <c r="D5" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="F5" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="G5" s="35">
+      <c r="G5" s="32">
         <v>2</v>
       </c>
-      <c r="H5" s="33" t="s">
+      <c r="H5" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="J5" s="33">
+      <c r="J5" s="8">
         <v>12</v>
       </c>
-      <c r="K5" s="33">
+      <c r="K5" s="8">
         <v>4</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="8">
         <v>12</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="8" t="s">
         <v>248</v>
       </c>
-      <c r="N5" s="34" t="s">
+      <c r="N5" s="31" t="s">
         <v>241</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="8">
         <v>23</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="P5" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="Q5" s="33">
+      <c r="Q5" s="8">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5">
+      <formula1>"Teroris,Korupsi,Narkotik,Kriminal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9">
+      <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P2:P5">
       <formula1>"Baik,Rusak"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N2:N5">
-      <formula1>"Teroris,Korupsi,Narkotik,Kriminal"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H12">
       <formula1>"Angka 8 (mulai kiri atas),Angka 8 (mulai kiri bawah),Angka 8 (mulai kanani atas),Angka 8 (mulai kanan bawah),Belakang Ke Depan (1 arah),Belakang Ke Depan (2 arah),Depan Ke Belakang (1 arah),Depan Ke Belakang (2 arah),Kanan Kiri (1 arah)"</formula1>
@@ -4365,17 +4382,14 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H7">
       <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
-      <formula1>"1,2,3,4"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F5">
       <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I9">
-      <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E5">
       <formula1>"Laki-laki,Perempuan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G5">
+      <formula1>"1,2,3,4"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D10">
       <formula1>"Umum,Mapenaling,Tutup Sunyi,Isolasi"</formula1>
@@ -4399,62 +4413,62 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.1484375" style="58" customWidth="1"/>
-    <col min="2" max="2" width="32.1484375" style="58" customWidth="1"/>
-    <col min="3" max="3" width="29.859375" style="58" customWidth="1"/>
-    <col min="4" max="4" width="27.1484375" style="59" customWidth="1"/>
-    <col min="5" max="5" width="32.4296875" style="59" customWidth="1"/>
-    <col min="6" max="6" width="42.0078125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="14.1484375" style="54" customWidth="1"/>
+    <col min="2" max="2" width="32.1484375" style="54" customWidth="1"/>
+    <col min="3" max="3" width="29.859375" style="54" customWidth="1"/>
+    <col min="4" max="4" width="27.1484375" style="55" customWidth="1"/>
+    <col min="5" max="5" width="32.4296875" style="55" customWidth="1"/>
+    <col min="6" max="6" width="42.0078125" style="54" customWidth="1"/>
     <col min="7" max="7" width="23.703125" customWidth="1"/>
     <col min="8" max="8" width="24.8671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="56" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="65" t="s">
+      <c r="E1" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="65" t="s">
+      <c r="F1" s="61" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="61" t="s">
+      <c r="G1" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="31" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" ht="19.5" customHeight="1" spans="1:9">
-      <c r="A2" s="63">
+      <c r="A2" s="59">
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="64" t="s">
+      <c r="D2" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="37" t="s">
+      <c r="E2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="37" t="s">
+      <c r="F2" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="8" t="s">
@@ -4472,16 +4486,16 @@
       <c r="B3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G3" s="8" t="s">
@@ -4499,16 +4513,16 @@
       <c r="B4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="64" t="s">
+      <c r="D4" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G4" s="8" t="s">
@@ -4526,16 +4540,16 @@
       <c r="B5" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E5" s="37" t="s">
+      <c r="E5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G5" s="8" t="s">
@@ -4553,16 +4567,16 @@
       <c r="B6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="C6" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="64" t="s">
+      <c r="D6" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="37" t="s">
+      <c r="E6" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G6" s="8" t="s">
@@ -4580,16 +4594,16 @@
       <c r="B7" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="37" t="s">
+      <c r="E7" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="37" t="s">
+      <c r="F7" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G7" s="8" t="s">
@@ -4607,16 +4621,16 @@
       <c r="B8" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="37" t="s">
+      <c r="E8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G8" s="8" t="s">
@@ -4634,16 +4648,16 @@
       <c r="B9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="64" t="s">
+      <c r="C9" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="37" t="s">
+      <c r="E9" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="37" t="s">
+      <c r="F9" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G9" s="8" t="s">
@@ -4661,16 +4675,16 @@
       <c r="B10" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="64" t="s">
+      <c r="C10" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="E10" s="37" t="s">
+      <c r="E10" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="33" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -4697,10 +4711,10 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="B1:Q6"/>
+  <dimension ref="B1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+      <selection activeCell="S33" sqref="S33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="5"/>
@@ -4720,9 +4734,14 @@
     <col min="15" max="15" width="27.734375" customWidth="1"/>
     <col min="16" max="16" width="24.34375" customWidth="1"/>
     <col min="17" max="17" width="21.875" customWidth="1"/>
+    <col min="18" max="18" width="14.578125" customWidth="1"/>
+    <col min="19" max="19" width="23.046875" customWidth="1"/>
+    <col min="20" max="20" width="17.0625" customWidth="1"/>
+    <col min="21" max="21" width="16.2734375" customWidth="1"/>
+    <col min="22" max="22" width="14.9765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.75" spans="2:17">
+    <row r="1" ht="14.75" spans="2:22">
       <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
@@ -4744,35 +4763,50 @@
       <c r="H1" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="M1" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="18" t="s">
         <v>255</v>
       </c>
-      <c r="O1" s="25" t="s">
+      <c r="O1" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="P1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="Q1" s="29" t="s">
+      <c r="Q1" s="18" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="2" spans="2:17">
+      <c r="R1" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="S1" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="T1" s="21" t="s">
+        <v>225</v>
+      </c>
+      <c r="U1" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="2:22">
       <c r="B2" s="3" t="s">
         <v>157</v>
       </c>
@@ -4791,38 +4825,53 @@
       <c r="G2" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="21">
+      <c r="L2" s="5">
         <v>2</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="N2" s="21" t="s">
+      <c r="N2" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="O2" s="21">
+      <c r="O2" s="5">
         <v>10</v>
       </c>
-      <c r="P2" s="26">
+      <c r="P2" s="5">
         <v>1</v>
       </c>
-      <c r="Q2" s="30">
+      <c r="Q2" s="22">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="2:17">
+      <c r="R2" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="T2" s="5">
+        <v>30</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="V2" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="2:22">
       <c r="B3" s="6" t="s">
         <v>167</v>
       </c>
@@ -4838,41 +4887,56 @@
       <c r="F3" s="8">
         <v>1</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="7" t="s">
         <v>234</v>
       </c>
-      <c r="L3" s="22">
+      <c r="L3" s="7">
         <v>1</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="O3" s="22">
+      <c r="O3" s="7">
         <v>15</v>
       </c>
-      <c r="P3" s="27">
+      <c r="P3" s="7">
         <v>2</v>
       </c>
-      <c r="Q3" s="31">
+      <c r="Q3" s="24">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="2:17">
+      <c r="R3" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="S3" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="T3" s="7">
+        <v>33</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="V3" s="30">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22">
       <c r="B4" s="6" t="s">
         <v>158</v>
       </c>
@@ -4888,41 +4952,56 @@
       <c r="F4" s="8">
         <v>3</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="H4" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="L4" s="22">
+      <c r="L4" s="7">
         <v>3</v>
       </c>
-      <c r="M4" s="22" t="s">
+      <c r="M4" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="N4" s="22" t="s">
+      <c r="N4" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="O4" s="22">
+      <c r="O4" s="7">
         <v>14</v>
       </c>
-      <c r="P4" s="27">
+      <c r="P4" s="7">
         <v>3</v>
       </c>
-      <c r="Q4" s="31">
+      <c r="Q4" s="24">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="2:17">
+      <c r="R4" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="S4" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="T4" s="7">
+        <v>43</v>
+      </c>
+      <c r="U4" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="V4" s="30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22">
       <c r="B5" s="6" t="s">
         <v>159</v>
       </c>
@@ -4938,41 +5017,56 @@
       <c r="F5" s="8">
         <v>1</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="14" t="s">
         <v>164</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="7" t="s">
         <v>163</v>
       </c>
-      <c r="J5" s="22" t="s">
+      <c r="J5" s="7" t="s">
         <v>245</v>
       </c>
-      <c r="K5" s="22" t="s">
+      <c r="K5" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="L5" s="22">
+      <c r="L5" s="7">
         <v>2</v>
       </c>
-      <c r="M5" s="22" t="s">
+      <c r="M5" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="N5" s="22" t="s">
+      <c r="N5" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="O5" s="22">
+      <c r="O5" s="7">
         <v>12</v>
       </c>
-      <c r="P5" s="27">
+      <c r="P5" s="7">
         <v>4</v>
       </c>
-      <c r="Q5" s="31">
+      <c r="Q5" s="24">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" ht="14.75" spans="2:17">
+      <c r="R5" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="S5" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="T5" s="7">
+        <v>23</v>
+      </c>
+      <c r="U5" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="V5" s="30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" ht="14.75" spans="2:22">
       <c r="B6" s="9" t="s">
         <v>51</v>
       </c>
@@ -4988,65 +5082,86 @@
       <c r="F6" s="10">
         <v>1</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="9" t="s">
         <v>259</v>
       </c>
-      <c r="I6" s="23" t="s">
+      <c r="I6" s="17" t="s">
         <v>163</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="K6" s="23" t="s">
+      <c r="K6" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="17">
         <v>2</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="17" t="s">
         <v>231</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="17">
         <v>12</v>
       </c>
-      <c r="P6" s="28">
+      <c r="P6" s="17">
         <v>5</v>
       </c>
-      <c r="Q6" s="32">
+      <c r="Q6" s="26">
         <v>15</v>
       </c>
+      <c r="R6" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="S6" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="T6" s="17">
+        <v>23</v>
+      </c>
+      <c r="U6" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="V6" s="15">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="9">
+  <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="U6 U2:U5">
+      <formula1>"Baik,Rusak"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S6 S2:S5">
+      <formula1>"Teroris,Korupsi,Narkotik,Kriminal"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6 N2:N5">
+      <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M6 M2:M5">
       <formula1>"Angka 8 mulai kiri atas,Angka 8 mulai kiri bawah,Angka 8 mulai kanani atas,Angka 8 mulai kanan bawah,Belakang Ke Depan 1 arah,Belakang Ke Depan 2 arah,Depan Ke Belakang 1 arah,Depan Ke Belakang 2 arah,Kanan Kiri 1 arah"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L6 L2:L5">
       <formula1>"1,2,3,4"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6 J2:J5">
+      <formula1>"Laki-laki,Perempuan"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6 E2:E5">
       <formula1>"Mapenaling,Umum,Tutup Sunyi,Isolasi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 K2:K5">
-      <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D2:D5">
+      <formula1>"Diizinkan,Perbaikan,Dalam Proses"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I6">
       <formula1>"Umum,Tutup Sunyi,Mapenaling,Isolasi"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N6 N2:N5">
-      <formula1>"Anak-anak,Dewasa,Lansia"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6 J2:J5">
-      <formula1>"Laki-laki,Perempuan"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6 D2:D5">
-      <formula1>"Diizinkan,Perbaikan,Dalam Proses"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6 K2:K5">
+      <formula1>"Korupsi,Teroris,Kriminal,Kriminal Teroris Korupsi,Korupsi Teroris,Teroris Kriminal"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B6 B2:B5">
       <formula1>"status,blok,jumlahlantai,semua,tipeblok"</formula1>
@@ -5075,7 +5190,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -5137,7 +5252,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -5208,33 +5323,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="53" t="s">
+      <c r="C1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="53" t="s">
+      <c r="D1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="53" t="s">
+      <c r="E1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="G1" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="53" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="41">
+      <c r="A2" s="37">
         <v>2</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -5255,12 +5370,12 @@
       <c r="G2" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="41"/>
+      <c r="A3" s="37"/>
       <c r="B3" s="8" t="s">
         <v>58</v>
       </c>
@@ -5279,12 +5394,12 @@
       <c r="G3" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="41"/>
+      <c r="A4" s="37"/>
       <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
@@ -5303,12 +5418,12 @@
       <c r="G4" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="15" t="s">
+      <c r="H4" s="14" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="41"/>
+      <c r="A5" s="37"/>
       <c r="B5" s="8" t="s">
         <v>50</v>
       </c>
@@ -5327,12 +5442,12 @@
       <c r="G5" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="14" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="41"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="8" t="s">
         <v>51</v>
       </c>
@@ -5351,12 +5466,12 @@
       <c r="G6" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="7" ht="14.75" spans="1:8">
-      <c r="A7" s="42"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="8">
@@ -5371,21 +5486,21 @@
       <c r="G7" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="44" t="s">
+      <c r="H7" s="40" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="11" ht="14.75"/>
     <row r="12" spans="1:1">
-      <c r="A12" s="54" t="s">
+      <c r="A12" s="50" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="56" t="s">
+      <c r="B13" s="52" t="s">
         <v>62</v>
       </c>
     </row>
@@ -5428,7 +5543,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>63</v>
       </c>
       <c r="B1" t="s">
@@ -5463,7 +5578,7 @@
       <c r="C2" t="s">
         <v>71</v>
       </c>
-      <c r="D2" s="51">
+      <c r="D2" s="47">
         <v>3434</v>
       </c>
       <c r="E2" t="s">
@@ -5571,52 +5686,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" s="46" t="s">
+      <c r="A1" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="C1" s="31" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="D1" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="E1" s="31" t="s">
         <v>83</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="31" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="36" t="s">
+      <c r="H1" s="31" t="s">
         <v>86</v>
       </c>
-      <c r="I1" s="36" t="s">
+      <c r="I1" s="31" t="s">
         <v>87</v>
       </c>
-      <c r="J1" s="36" t="s">
+      <c r="J1" s="31" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="46">
+      <c r="A2" s="42">
         <v>5</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="43" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
-      <c r="H2" s="47" t="s">
+      <c r="H2" s="43" t="s">
         <v>91</v>
       </c>
       <c r="I2" s="8"/>
@@ -5627,14 +5742,14 @@
       <c r="B3" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="43" t="s">
         <v>71</v>
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="43" t="s">
         <v>91</v>
       </c>
       <c r="I3" s="8"/>
@@ -5645,20 +5760,20 @@
       <c r="B4" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="47" t="s">
+      <c r="C4" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D4" s="47">
+      <c r="D4" s="43">
         <v>3460</v>
       </c>
-      <c r="E4" s="47" t="s">
+      <c r="E4" s="43" t="s">
         <v>93</v>
       </c>
-      <c r="F4" s="47" t="s">
+      <c r="F4" s="43" t="s">
         <v>94</v>
       </c>
       <c r="G4" s="8"/>
-      <c r="H4" s="47" t="s">
+      <c r="H4" s="43" t="s">
         <v>91</v>
       </c>
       <c r="I4" s="8"/>
@@ -5669,22 +5784,22 @@
       <c r="B5" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="47" t="s">
+      <c r="C5" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="D5" s="47">
+      <c r="D5" s="43">
         <v>123</v>
       </c>
-      <c r="E5" s="47" t="s">
+      <c r="E5" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="47" t="s">
+      <c r="F5" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="G5" s="47" t="s">
+      <c r="G5" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="H5" s="47" t="s">
+      <c r="H5" s="43" t="s">
         <v>97</v>
       </c>
       <c r="I5" s="8"/>
@@ -5806,13 +5921,13 @@
       <c r="A17" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="44"/>
     </row>
     <row r="18" ht="14.75" spans="1:2">
       <c r="A18" t="s">
         <v>99</v>
       </c>
-      <c r="B18" s="49"/>
+      <c r="B18" s="45"/>
     </row>
   </sheetData>
   <dataValidations count="2">
@@ -5878,7 +5993,7 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2" s="45" t="s">
+      <c r="F2" s="41" t="s">
         <v>106</v>
       </c>
       <c r="G2" t="s">

</xml_diff>